<commit_message>
Removed Driver Quit, Updated BuyerProcess datasheet
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/BuyerProcess.xlsx
+++ b/src/test/resources/datasheets/BuyerProcess.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Buyer" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Suggested Supplier(s)</t>
   </si>
@@ -106,6 +107,30 @@
   </si>
   <si>
     <t>Desktops</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Description </t>
+  </si>
+  <si>
+    <t>UNSPSC Code</t>
+  </si>
+  <si>
+    <t>REQUESTOR</t>
+  </si>
+  <si>
+    <t>XEEVA -MJ</t>
+  </si>
+  <si>
+    <t>REPOFLOR 100 MG</t>
+  </si>
+  <si>
+    <t>UNSPSC001</t>
   </si>
 </sst>
 </file>
@@ -437,105 +462,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>